<commit_message>
Análisis de instrucciones y Testbench
Análisis de instrucciones y definición de instrucciones implementadas en
documento WORD.

Trabajo sobre señales de control en EXCEL.

Testbench de BrAdder, y Control principal, de este ultimo solo se
identifica el tipo de instrucción.
</commit_message>
<xml_diff>
--- a/PDFs/Instrucciones implementadas.xlsx
+++ b/PDFs/Instrucciones implementadas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18855" windowHeight="11760" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="18855" windowHeight="11760" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="5" r:id="rId1"/>
@@ -411,9 +411,6 @@
     <t>1111001010100001</t>
   </si>
   <si>
-    <t>1111001000000000</t>
-  </si>
-  <si>
     <t>1111001011000000</t>
   </si>
   <si>
@@ -439,6 +436,9 @@
   </si>
   <si>
     <t>1001000110000000</t>
+  </si>
+  <si>
+    <t>1111001001000000</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,6 +498,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -691,21 +697,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -729,6 +720,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1028,7 +1042,7 @@
   <dimension ref="B2:AH18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="M6" sqref="M6:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1160,98 +1174,98 @@
       <c r="G3" s="5">
         <v>0</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
       <c r="S3" s="5">
         <v>0</v>
       </c>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="23"/>
-      <c r="AH3" s="23"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
     </row>
     <row r="4" spans="2:34">
-      <c r="B4" t="s">
+      <c r="B4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="1" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="22" t="s">
+      <c r="I4" s="36">
+        <v>0</v>
+      </c>
+      <c r="J4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="1" t="s">
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22" t="s">
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22" t="s">
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22" t="s">
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="38"/>
     </row>
     <row r="5" spans="2:34">
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
       <c r="H5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1267,48 +1281,48 @@
       <c r="L5" s="1">
         <v>0</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22" t="s">
+      <c r="N5" s="37"/>
+      <c r="O5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22" t="s">
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="22" t="s">
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="X5" s="22"/>
-      <c r="Y5" s="22"/>
-      <c r="Z5" s="22"/>
-      <c r="AA5" s="22" t="s">
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
+      <c r="AA5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AB5" s="22"/>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="22"/>
-      <c r="AE5" s="22"/>
-      <c r="AF5" s="22"/>
-      <c r="AG5" s="22"/>
-      <c r="AH5" s="22"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37"/>
+      <c r="AD5" s="37"/>
+      <c r="AE5" s="37"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="37"/>
+      <c r="AH5" s="37"/>
     </row>
     <row r="6" spans="2:34">
       <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1324,38 +1338,38 @@
       <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="M6" s="22" t="s">
+      <c r="M6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22" t="s">
+      <c r="N6" s="37"/>
+      <c r="O6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22" t="s">
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="22"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22" t="s">
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22" t="s">
+      <c r="X6" s="37"/>
+      <c r="Y6" s="37"/>
+      <c r="Z6" s="37"/>
+      <c r="AA6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="22"/>
-      <c r="AG6" s="22"/>
-      <c r="AH6" s="22"/>
+      <c r="AB6" s="37"/>
+      <c r="AC6" s="37"/>
+      <c r="AD6" s="37"/>
+      <c r="AE6" s="37"/>
+      <c r="AF6" s="37"/>
+      <c r="AG6" s="37"/>
+      <c r="AH6" s="37"/>
     </row>
     <row r="7" spans="2:34">
       <c r="T7" s="3"/>
@@ -1397,88 +1411,88 @@
       <c r="I8" s="5">
         <v>1</v>
       </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="23"/>
-      <c r="AG8" s="23"/>
-      <c r="AH8" s="23"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="39"/>
+      <c r="Y8" s="39"/>
+      <c r="Z8" s="39"/>
+      <c r="AA8" s="39"/>
+      <c r="AB8" s="39"/>
+      <c r="AC8" s="39"/>
+      <c r="AD8" s="39"/>
+      <c r="AE8" s="39"/>
+      <c r="AF8" s="39"/>
+      <c r="AG8" s="39"/>
+      <c r="AH8" s="39"/>
     </row>
     <row r="9" spans="2:34">
       <c r="B9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="1">
         <v>0</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22" t="s">
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
       <c r="N9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O9" s="22" t="s">
+      <c r="O9" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
       <c r="S9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="T9" s="22" t="s">
+      <c r="T9" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="22" t="s">
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="X9" s="22"/>
-      <c r="Y9" s="22"/>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="22" t="s">
+      <c r="X9" s="37"/>
+      <c r="Y9" s="37"/>
+      <c r="Z9" s="37"/>
+      <c r="AA9" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="AB9" s="22"/>
-      <c r="AC9" s="22" t="s">
+      <c r="AB9" s="37"/>
+      <c r="AC9" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="AD9" s="22"/>
-      <c r="AE9" s="22" t="s">
+      <c r="AD9" s="37"/>
+      <c r="AE9" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AF9" s="22"/>
-      <c r="AG9" s="22"/>
-      <c r="AH9" s="22"/>
+      <c r="AF9" s="37"/>
+      <c r="AG9" s="37"/>
+      <c r="AH9" s="37"/>
     </row>
     <row r="11" spans="2:34">
       <c r="B11" s="4" t="s">
@@ -1505,98 +1519,98 @@
       <c r="I11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="23"/>
-      <c r="AE11" s="23"/>
-      <c r="AF11" s="23"/>
-      <c r="AG11" s="23"/>
-      <c r="AH11" s="23"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="39"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="39"/>
+      <c r="W11" s="39"/>
+      <c r="X11" s="39"/>
+      <c r="Y11" s="39"/>
+      <c r="Z11" s="39"/>
+      <c r="AA11" s="39"/>
+      <c r="AB11" s="39"/>
+      <c r="AC11" s="39"/>
+      <c r="AD11" s="39"/>
+      <c r="AE11" s="39"/>
+      <c r="AF11" s="39"/>
+      <c r="AG11" s="39"/>
+      <c r="AH11" s="39"/>
     </row>
     <row r="12" spans="2:34">
       <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
       <c r="J12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="K12" s="1">
         <v>1</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="L12" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="M12" s="22"/>
+      <c r="M12" s="37"/>
       <c r="N12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O12" s="22" t="s">
+      <c r="O12" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22" t="s">
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="T12" s="22"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="22"/>
-      <c r="W12" s="22" t="s">
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="22"/>
-      <c r="AA12" s="22"/>
-      <c r="AB12" s="22"/>
-      <c r="AC12" s="22"/>
-      <c r="AD12" s="22"/>
-      <c r="AE12" s="22"/>
-      <c r="AF12" s="22"/>
-      <c r="AG12" s="22"/>
-      <c r="AH12" s="22"/>
+      <c r="X12" s="37"/>
+      <c r="Y12" s="37"/>
+      <c r="Z12" s="37"/>
+      <c r="AA12" s="37"/>
+      <c r="AB12" s="37"/>
+      <c r="AC12" s="37"/>
+      <c r="AD12" s="37"/>
+      <c r="AE12" s="37"/>
+      <c r="AF12" s="37"/>
+      <c r="AG12" s="37"/>
+      <c r="AH12" s="37"/>
     </row>
     <row r="13" spans="2:34">
       <c r="B13" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K13" s="22"/>
+      <c r="K13" s="37"/>
       <c r="L13" s="1">
         <v>0</v>
       </c>
@@ -1606,42 +1620,42 @@
       <c r="N13" s="1">
         <v>1</v>
       </c>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="22"/>
-      <c r="U13" s="22"/>
-      <c r="V13" s="22"/>
-      <c r="W13" s="22"/>
-      <c r="X13" s="22"/>
-      <c r="Y13" s="22"/>
-      <c r="Z13" s="22"/>
-      <c r="AA13" s="22"/>
-      <c r="AB13" s="22"/>
-      <c r="AC13" s="22"/>
-      <c r="AD13" s="22"/>
-      <c r="AE13" s="22"/>
-      <c r="AF13" s="22"/>
-      <c r="AG13" s="22"/>
-      <c r="AH13" s="22"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
+      <c r="Y13" s="37"/>
+      <c r="Z13" s="37"/>
+      <c r="AA13" s="37"/>
+      <c r="AB13" s="37"/>
+      <c r="AC13" s="37"/>
+      <c r="AD13" s="37"/>
+      <c r="AE13" s="37"/>
+      <c r="AF13" s="37"/>
+      <c r="AG13" s="37"/>
+      <c r="AH13" s="37"/>
     </row>
     <row r="14" spans="2:34">
       <c r="B14" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
       <c r="J14" s="1">
         <v>0</v>
       </c>
-      <c r="K14" s="22"/>
+      <c r="K14" s="37"/>
       <c r="L14" s="1">
         <v>1</v>
       </c>
@@ -1651,26 +1665,26 @@
       <c r="N14" s="1">
         <v>0</v>
       </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
-      <c r="U14" s="22"/>
-      <c r="V14" s="22"/>
-      <c r="W14" s="22"/>
-      <c r="X14" s="22"/>
-      <c r="Y14" s="22"/>
-      <c r="Z14" s="22"/>
-      <c r="AA14" s="22"/>
-      <c r="AB14" s="22"/>
-      <c r="AC14" s="22"/>
-      <c r="AD14" s="22"/>
-      <c r="AE14" s="22"/>
-      <c r="AF14" s="22"/>
-      <c r="AG14" s="22"/>
-      <c r="AH14" s="22"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="37"/>
+      <c r="Z14" s="37"/>
+      <c r="AA14" s="37"/>
+      <c r="AB14" s="37"/>
+      <c r="AC14" s="37"/>
+      <c r="AD14" s="37"/>
+      <c r="AE14" s="37"/>
+      <c r="AF14" s="37"/>
+      <c r="AG14" s="37"/>
+      <c r="AH14" s="37"/>
     </row>
     <row r="16" spans="2:34">
       <c r="B16" s="4" t="s">
@@ -1691,61 +1705,61 @@
       <c r="G16" s="5">
         <v>0</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
       <c r="S16" s="5">
         <v>1</v>
       </c>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="23"/>
-      <c r="AE16" s="23"/>
-      <c r="AF16" s="23"/>
-      <c r="AG16" s="23"/>
-      <c r="AH16" s="23"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="39"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="39"/>
+      <c r="Z16" s="39"/>
+      <c r="AA16" s="39"/>
+      <c r="AB16" s="39"/>
+      <c r="AC16" s="39"/>
+      <c r="AD16" s="39"/>
+      <c r="AE16" s="39"/>
+      <c r="AF16" s="39"/>
+      <c r="AG16" s="39"/>
+      <c r="AH16" s="39"/>
     </row>
     <row r="17" spans="2:34">
       <c r="B17" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
       <c r="H17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
       <c r="T17" s="1">
         <v>0</v>
       </c>
@@ -1758,47 +1772,47 @@
       <c r="W17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="X17" s="22" t="s">
+      <c r="X17" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="Y17" s="22"/>
-      <c r="Z17" s="22"/>
-      <c r="AA17" s="22"/>
-      <c r="AB17" s="22"/>
-      <c r="AC17" s="22"/>
-      <c r="AD17" s="22"/>
-      <c r="AE17" s="22"/>
-      <c r="AF17" s="22"/>
-      <c r="AG17" s="22"/>
-      <c r="AH17" s="22"/>
+      <c r="Y17" s="37"/>
+      <c r="Z17" s="37"/>
+      <c r="AA17" s="37"/>
+      <c r="AB17" s="37"/>
+      <c r="AC17" s="37"/>
+      <c r="AD17" s="37"/>
+      <c r="AE17" s="37"/>
+      <c r="AF17" s="37"/>
+      <c r="AG17" s="37"/>
+      <c r="AH17" s="37"/>
     </row>
     <row r="18" spans="2:34">
       <c r="B18" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
       <c r="H18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22" t="s">
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
       <c r="T18" s="1">
         <v>0</v>
       </c>
@@ -1811,38 +1825,34 @@
       <c r="W18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="X18" s="22" t="s">
+      <c r="X18" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="Y18" s="22"/>
-      <c r="Z18" s="22"/>
-      <c r="AA18" s="22"/>
-      <c r="AB18" s="22"/>
-      <c r="AC18" s="22"/>
-      <c r="AD18" s="22"/>
-      <c r="AE18" s="22"/>
-      <c r="AF18" s="22"/>
-      <c r="AG18" s="22"/>
-      <c r="AH18" s="22"/>
+      <c r="Y18" s="37"/>
+      <c r="Z18" s="37"/>
+      <c r="AA18" s="37"/>
+      <c r="AB18" s="37"/>
+      <c r="AC18" s="37"/>
+      <c r="AD18" s="37"/>
+      <c r="AE18" s="37"/>
+      <c r="AF18" s="37"/>
+      <c r="AG18" s="37"/>
+      <c r="AH18" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="H3:R3"/>
-    <mergeCell ref="T3:AH3"/>
-    <mergeCell ref="C4:G6"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="S4:S6"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="AA4:AH4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:R5"/>
+  <mergeCells count="49">
     <mergeCell ref="T5:V5"/>
     <mergeCell ref="W5:Z5"/>
     <mergeCell ref="AA5:AH5"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="O6:R6"/>
+    <mergeCell ref="H3:R3"/>
+    <mergeCell ref="T3:AH3"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="AA4:AH4"/>
     <mergeCell ref="T6:V6"/>
     <mergeCell ref="W6:Z6"/>
     <mergeCell ref="AA6:AH6"/>
@@ -1859,22 +1869,27 @@
     <mergeCell ref="X18:AH18"/>
     <mergeCell ref="J11:AH11"/>
     <mergeCell ref="L12:M12"/>
+    <mergeCell ref="C12:I14"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="H16:R16"/>
+    <mergeCell ref="T16:AH16"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="S13:V14"/>
+    <mergeCell ref="W13:AH14"/>
+    <mergeCell ref="W9:Z9"/>
     <mergeCell ref="O12:R12"/>
     <mergeCell ref="S12:V12"/>
     <mergeCell ref="W12:AH12"/>
     <mergeCell ref="K13:K14"/>
     <mergeCell ref="O13:R14"/>
-    <mergeCell ref="H16:R16"/>
-    <mergeCell ref="T16:AH16"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="S13:V14"/>
-    <mergeCell ref="W13:AH14"/>
+    <mergeCell ref="C5:G6"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="S5:S6"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="J9:M9"/>
-    <mergeCell ref="C12:I14"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="W9:Z9"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1885,7 +1900,7 @@
   <dimension ref="B2:AV42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6:AH6"/>
+      <selection activeCell="C16" sqref="C16:AH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2030,88 +2045,88 @@
       <c r="G3" s="5">
         <v>0</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
       <c r="S3" s="5">
         <v>0</v>
       </c>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="23"/>
-      <c r="AH3" s="23"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
     </row>
     <row r="4" spans="2:37">
-      <c r="B4" t="s">
+      <c r="B4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="1" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="22" t="s">
+      <c r="I4" s="36">
+        <v>0</v>
+      </c>
+      <c r="J4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="1" t="s">
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22" t="s">
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22" t="s">
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22" t="s">
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="38"/>
       <c r="AJ4" t="s">
         <v>4</v>
       </c>
@@ -2123,11 +2138,11 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
       <c r="H5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2143,38 +2158,38 @@
       <c r="L5" s="1">
         <v>0</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22" t="s">
+      <c r="N5" s="37"/>
+      <c r="O5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22" t="s">
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="22" t="s">
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="X5" s="22"/>
-      <c r="Y5" s="22"/>
-      <c r="Z5" s="22"/>
-      <c r="AA5" s="22" t="s">
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
+      <c r="AA5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AB5" s="22"/>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="22"/>
-      <c r="AE5" s="22"/>
-      <c r="AF5" s="22"/>
-      <c r="AG5" s="22"/>
-      <c r="AH5" s="22"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37"/>
+      <c r="AD5" s="37"/>
+      <c r="AE5" s="37"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="37"/>
+      <c r="AH5" s="37"/>
       <c r="AK5" t="s">
         <v>15</v>
       </c>
@@ -2183,11 +2198,11 @@
       <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2203,38 +2218,38 @@
       <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="M6" s="22" t="s">
+      <c r="M6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22" t="s">
+      <c r="N6" s="37"/>
+      <c r="O6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22" t="s">
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="22"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22" t="s">
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22" t="s">
+      <c r="X6" s="37"/>
+      <c r="Y6" s="37"/>
+      <c r="Z6" s="37"/>
+      <c r="AA6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="22"/>
-      <c r="AG6" s="22"/>
-      <c r="AH6" s="22"/>
+      <c r="AB6" s="37"/>
+      <c r="AC6" s="37"/>
+      <c r="AD6" s="37"/>
+      <c r="AE6" s="37"/>
+      <c r="AF6" s="37"/>
+      <c r="AG6" s="37"/>
+      <c r="AH6" s="37"/>
       <c r="AK6" t="s">
         <v>16</v>
       </c>
@@ -2336,37 +2351,37 @@
       <c r="G13" s="6">
         <v>0</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="36"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
       <c r="S13" s="6">
         <v>0</v>
       </c>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
-      <c r="Y13" s="30"/>
-      <c r="Z13" s="30"/>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35"/>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35"/>
-      <c r="AE13" s="35"/>
-      <c r="AF13" s="35"/>
-      <c r="AG13" s="35"/>
-      <c r="AH13" s="35"/>
-      <c r="AI13" s="33"/>
-      <c r="AJ13" s="34"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25"/>
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30"/>
+      <c r="AC13" s="30"/>
+      <c r="AD13" s="30"/>
+      <c r="AE13" s="30"/>
+      <c r="AF13" s="30"/>
+      <c r="AG13" s="30"/>
+      <c r="AH13" s="30"/>
+      <c r="AI13" s="28"/>
+      <c r="AJ13" s="29"/>
     </row>
     <row r="14" spans="2:37">
       <c r="C14" s="2"/>
@@ -2374,8 +2389,8 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -2401,8 +2416,8 @@
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
-      <c r="AI14" s="33"/>
-      <c r="AJ14" s="34"/>
+      <c r="AI14" s="28"/>
+      <c r="AJ14" s="29"/>
     </row>
     <row r="15" spans="2:37">
       <c r="B15" t="s">
@@ -2423,10 +2438,10 @@
       <c r="G15" s="6">
         <v>0</v>
       </c>
-      <c r="H15" s="35">
-        <v>0</v>
-      </c>
-      <c r="I15" s="36">
+      <c r="H15" s="30">
+        <v>0</v>
+      </c>
+      <c r="I15" s="31">
         <v>1</v>
       </c>
       <c r="J15" s="2">
@@ -2444,70 +2459,70 @@
       <c r="N15" s="2">
         <v>0</v>
       </c>
-      <c r="O15" s="32">
-        <v>0</v>
-      </c>
-      <c r="P15" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="32">
-        <v>0</v>
-      </c>
-      <c r="R15" s="32">
+      <c r="O15" s="27">
+        <v>0</v>
+      </c>
+      <c r="P15" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="27">
+        <v>0</v>
+      </c>
+      <c r="R15" s="27">
         <v>1</v>
       </c>
       <c r="S15" s="6">
         <v>0</v>
       </c>
-      <c r="T15" s="35">
-        <v>0</v>
-      </c>
-      <c r="U15" s="35">
-        <v>0</v>
-      </c>
-      <c r="V15" s="35">
-        <v>0</v>
-      </c>
-      <c r="W15" s="30">
-        <v>0</v>
-      </c>
-      <c r="X15" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="30">
-        <v>1</v>
-      </c>
-      <c r="AA15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="35">
-        <v>1</v>
-      </c>
-      <c r="AG15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="33" t="s">
+      <c r="T15" s="30">
+        <v>0</v>
+      </c>
+      <c r="U15" s="30">
+        <v>0</v>
+      </c>
+      <c r="V15" s="30">
+        <v>0</v>
+      </c>
+      <c r="W15" s="25">
+        <v>0</v>
+      </c>
+      <c r="X15" s="25">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="30">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="AJ15" s="34" t="s">
+      <c r="AJ15" s="29" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2530,10 +2545,10 @@
       <c r="G16" s="6">
         <v>0</v>
       </c>
-      <c r="H16" s="35">
-        <v>0</v>
-      </c>
-      <c r="I16" s="36">
+      <c r="H16" s="30">
+        <v>0</v>
+      </c>
+      <c r="I16" s="31">
         <v>1</v>
       </c>
       <c r="J16" s="2">
@@ -2551,215 +2566,215 @@
       <c r="N16" s="2">
         <v>0</v>
       </c>
-      <c r="O16" s="32">
-        <v>0</v>
-      </c>
-      <c r="P16" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="32">
-        <v>0</v>
-      </c>
-      <c r="R16" s="32">
+      <c r="O16" s="27">
+        <v>0</v>
+      </c>
+      <c r="P16" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="27">
+        <v>0</v>
+      </c>
+      <c r="R16" s="27">
         <v>1</v>
       </c>
       <c r="S16" s="6">
         <v>0</v>
       </c>
-      <c r="T16" s="35">
-        <v>0</v>
-      </c>
-      <c r="U16" s="35">
-        <v>0</v>
-      </c>
-      <c r="V16" s="35">
-        <v>0</v>
-      </c>
-      <c r="W16" s="30">
-        <v>0</v>
-      </c>
-      <c r="X16" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="30">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="35">
-        <v>1</v>
-      </c>
-      <c r="AF16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="33" t="s">
+      <c r="T16" s="30">
+        <v>0</v>
+      </c>
+      <c r="U16" s="30">
+        <v>0</v>
+      </c>
+      <c r="V16" s="30">
+        <v>0</v>
+      </c>
+      <c r="W16" s="25">
+        <v>0</v>
+      </c>
+      <c r="X16" s="25">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="30">
+        <v>1</v>
+      </c>
+      <c r="AF16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="AJ16" s="34" t="s">
-        <v>126</v>
+      <c r="AJ16" s="29" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="2:42">
-      <c r="B17" s="37"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="36"/>
-      <c r="W17" s="36"/>
-      <c r="X17" s="36"/>
-      <c r="Y17" s="36"/>
-      <c r="Z17" s="36"/>
-      <c r="AA17" s="36"/>
-      <c r="AB17" s="36"/>
-      <c r="AC17" s="36"/>
-      <c r="AD17" s="36"/>
-      <c r="AE17" s="36"/>
-      <c r="AF17" s="36"/>
-      <c r="AG17" s="36"/>
-      <c r="AH17" s="36"/>
-      <c r="AI17" s="33"/>
-      <c r="AJ17" s="34"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="31"/>
+      <c r="Y17" s="31"/>
+      <c r="Z17" s="31"/>
+      <c r="AA17" s="31"/>
+      <c r="AB17" s="31"/>
+      <c r="AC17" s="31"/>
+      <c r="AD17" s="31"/>
+      <c r="AE17" s="31"/>
+      <c r="AF17" s="31"/>
+      <c r="AG17" s="31"/>
+      <c r="AH17" s="31"/>
+      <c r="AI17" s="28"/>
+      <c r="AJ17" s="29"/>
     </row>
     <row r="18" spans="2:42">
       <c r="B18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="30">
+        <v>0</v>
+      </c>
+      <c r="I18" s="31">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+      <c r="O18" s="30">
+        <v>0</v>
+      </c>
+      <c r="P18" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="30">
+        <v>0</v>
+      </c>
+      <c r="R18" s="30">
+        <v>0</v>
+      </c>
+      <c r="S18" s="6">
+        <v>0</v>
+      </c>
+      <c r="T18" s="30">
+        <v>0</v>
+      </c>
+      <c r="U18" s="30">
+        <v>0</v>
+      </c>
+      <c r="V18" s="30">
+        <v>0</v>
+      </c>
+      <c r="W18" s="25">
+        <v>0</v>
+      </c>
+      <c r="X18" s="25">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="30">
+        <v>1</v>
+      </c>
+      <c r="AF18" s="30">
+        <v>1</v>
+      </c>
+      <c r="AG18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="30">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ18" s="29" t="s">
         <v>124</v>
-      </c>
-      <c r="C18" s="6">
-        <v>1</v>
-      </c>
-      <c r="D18" s="6">
-        <v>1</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1</v>
-      </c>
-      <c r="G18" s="6">
-        <v>0</v>
-      </c>
-      <c r="H18" s="35">
-        <v>0</v>
-      </c>
-      <c r="I18" s="36">
-        <v>1</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2">
-        <v>0</v>
-      </c>
-      <c r="L18" s="2">
-        <v>0</v>
-      </c>
-      <c r="M18" s="2">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2">
-        <v>0</v>
-      </c>
-      <c r="O18" s="35">
-        <v>0</v>
-      </c>
-      <c r="P18" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="35">
-        <v>0</v>
-      </c>
-      <c r="R18" s="35">
-        <v>0</v>
-      </c>
-      <c r="S18" s="6">
-        <v>0</v>
-      </c>
-      <c r="T18" s="35">
-        <v>0</v>
-      </c>
-      <c r="U18" s="35">
-        <v>0</v>
-      </c>
-      <c r="V18" s="35">
-        <v>0</v>
-      </c>
-      <c r="W18" s="30">
-        <v>0</v>
-      </c>
-      <c r="X18" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="30">
-        <v>1</v>
-      </c>
-      <c r="AA18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="35">
-        <v>1</v>
-      </c>
-      <c r="AF18" s="35">
-        <v>1</v>
-      </c>
-      <c r="AG18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AH18" s="35">
-        <v>1</v>
-      </c>
-      <c r="AI18" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="AJ18" s="34" t="s">
-        <v>125</v>
       </c>
       <c r="AK18" s="8"/>
     </row>
@@ -2782,10 +2797,10 @@
       <c r="G19" s="6">
         <v>0</v>
       </c>
-      <c r="H19" s="35">
-        <v>0</v>
-      </c>
-      <c r="I19" s="36">
+      <c r="H19" s="30">
+        <v>0</v>
+      </c>
+      <c r="I19" s="31">
         <v>1</v>
       </c>
       <c r="J19" s="2">
@@ -2803,73 +2818,73 @@
       <c r="N19" s="2">
         <v>0</v>
       </c>
-      <c r="O19" s="35">
-        <v>0</v>
-      </c>
-      <c r="P19" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="35">
-        <v>0</v>
-      </c>
-      <c r="R19" s="35">
+      <c r="O19" s="30">
+        <v>0</v>
+      </c>
+      <c r="P19" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="30">
+        <v>0</v>
+      </c>
+      <c r="R19" s="30">
         <v>0</v>
       </c>
       <c r="S19" s="6">
         <v>0</v>
       </c>
-      <c r="T19" s="35">
-        <v>0</v>
-      </c>
-      <c r="U19" s="35">
-        <v>0</v>
-      </c>
-      <c r="V19" s="35">
-        <v>0</v>
-      </c>
-      <c r="W19" s="30">
-        <v>0</v>
-      </c>
-      <c r="X19" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="30">
-        <v>1</v>
-      </c>
-      <c r="AA19" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE19" s="35">
-        <v>1</v>
-      </c>
-      <c r="AF19" s="35">
-        <v>1</v>
-      </c>
-      <c r="AG19" s="35">
-        <v>1</v>
-      </c>
-      <c r="AH19" s="35">
-        <v>1</v>
-      </c>
-      <c r="AI19" s="33" t="s">
+      <c r="T19" s="30">
+        <v>0</v>
+      </c>
+      <c r="U19" s="30">
+        <v>0</v>
+      </c>
+      <c r="V19" s="30">
+        <v>0</v>
+      </c>
+      <c r="W19" s="25">
+        <v>0</v>
+      </c>
+      <c r="X19" s="25">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="25">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="30">
+        <v>1</v>
+      </c>
+      <c r="AF19" s="30">
+        <v>1</v>
+      </c>
+      <c r="AG19" s="30">
+        <v>1</v>
+      </c>
+      <c r="AH19" s="30">
+        <v>1</v>
+      </c>
+      <c r="AI19" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="AJ19" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="AJ19" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="AK19" s="34"/>
+      <c r="AK19" s="29"/>
     </row>
     <row r="20" spans="2:42">
       <c r="O20" s="2"/>
@@ -2882,7 +2897,7 @@
     <row r="22" spans="2:42">
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
-      <c r="V22" s="38"/>
+      <c r="V22" s="33"/>
     </row>
     <row r="23" spans="2:42" ht="15.75" thickBot="1">
       <c r="O23" s="2"/>
@@ -2891,15 +2906,15 @@
     <row r="24" spans="2:42" ht="15.75" thickBot="1">
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
-      <c r="AJ24" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK24" s="25"/>
-      <c r="AL24" s="25"/>
-      <c r="AM24" s="25"/>
-      <c r="AN24" s="25"/>
-      <c r="AO24" s="25"/>
-      <c r="AP24" s="26"/>
+      <c r="AJ24" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK24" s="41"/>
+      <c r="AL24" s="41"/>
+      <c r="AM24" s="41"/>
+      <c r="AN24" s="41"/>
+      <c r="AO24" s="41"/>
+      <c r="AP24" s="42"/>
     </row>
     <row r="25" spans="2:42" ht="15.75" thickBot="1">
       <c r="O25" s="2"/>
@@ -3084,13 +3099,13 @@
       <c r="AO33" s="1"/>
     </row>
     <row r="34" spans="36:41" ht="15.75" thickBot="1">
-      <c r="AJ34" s="24" t="s">
+      <c r="AJ34" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="AK34" s="25"/>
-      <c r="AL34" s="25"/>
-      <c r="AM34" s="25"/>
-      <c r="AN34" s="26"/>
+      <c r="AK34" s="41"/>
+      <c r="AL34" s="41"/>
+      <c r="AM34" s="41"/>
+      <c r="AN34" s="42"/>
       <c r="AO34" s="1"/>
     </row>
     <row r="35" spans="36:41" ht="15.75" thickBot="1">
@@ -3154,13 +3169,13 @@
       <c r="AO38" s="1"/>
     </row>
     <row r="39" spans="36:41" ht="15.75" thickBot="1">
-      <c r="AJ39" s="24" t="s">
+      <c r="AJ39" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="AK39" s="25"/>
-      <c r="AL39" s="25"/>
-      <c r="AM39" s="25"/>
-      <c r="AN39" s="26"/>
+      <c r="AK39" s="41"/>
+      <c r="AL39" s="41"/>
+      <c r="AM39" s="41"/>
+      <c r="AN39" s="42"/>
       <c r="AO39" s="1"/>
     </row>
     <row r="40" spans="36:41" ht="15.75" thickBot="1">
@@ -3218,7 +3233,10 @@
       <c r="AO42" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="C5:G6"/>
+    <mergeCell ref="C4:G4"/>
     <mergeCell ref="AJ39:AN39"/>
     <mergeCell ref="H3:R3"/>
     <mergeCell ref="T3:AH3"/>
@@ -3227,8 +3245,7 @@
     <mergeCell ref="W4:Z4"/>
     <mergeCell ref="AA4:AH4"/>
     <mergeCell ref="AJ34:AN34"/>
-    <mergeCell ref="C4:G6"/>
-    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="S5:S6"/>
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="AJ24:AP24"/>
@@ -3240,7 +3257,6 @@
     <mergeCell ref="T6:V6"/>
     <mergeCell ref="W6:Z6"/>
     <mergeCell ref="AA6:AH6"/>
-    <mergeCell ref="J4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3251,8 +3267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AT28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AJ6" sqref="AJ6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3397,88 +3413,88 @@
       <c r="I3" s="5">
         <v>1</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="23"/>
-      <c r="AH3" s="23"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
     </row>
     <row r="4" spans="2:42">
       <c r="B4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22" t="s">
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
       <c r="N4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
       <c r="S4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="22" t="s">
+      <c r="T4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22" t="s">
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22" t="s">
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22" t="s">
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22" t="s">
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
       <c r="AJ4" t="s">
         <v>93</v>
       </c>
@@ -3529,15 +3545,15 @@
     </row>
     <row r="9" spans="2:42" ht="15.75" thickBot="1"/>
     <row r="10" spans="2:42" ht="15.75" thickBot="1">
-      <c r="AJ10" s="24" t="s">
+      <c r="AJ10" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="AK10" s="25"/>
-      <c r="AL10" s="25"/>
-      <c r="AM10" s="25"/>
-      <c r="AN10" s="25"/>
-      <c r="AO10" s="25"/>
-      <c r="AP10" s="26"/>
+      <c r="AK10" s="41"/>
+      <c r="AL10" s="41"/>
+      <c r="AM10" s="41"/>
+      <c r="AN10" s="41"/>
+      <c r="AO10" s="41"/>
+      <c r="AP10" s="42"/>
     </row>
     <row r="11" spans="2:42" ht="15.75" thickBot="1">
       <c r="AJ11" s="17" t="s">
@@ -3787,7 +3803,6 @@
       <c r="AF21" s="3"/>
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
-      <c r="AJ21" s="1"/>
       <c r="AL21" s="1"/>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
@@ -3825,7 +3840,6 @@
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
-      <c r="AJ22" s="1"/>
       <c r="AL22" s="1"/>
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
@@ -3836,7 +3850,6 @@
       <c r="AT22"/>
     </row>
     <row r="23" spans="3:46">
-      <c r="AJ23" s="1"/>
       <c r="AL23" s="1"/>
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
@@ -3847,7 +3860,6 @@
       <c r="AT23"/>
     </row>
     <row r="24" spans="3:46">
-      <c r="AJ24" s="1"/>
       <c r="AL24" s="1"/>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
@@ -3858,7 +3870,6 @@
       <c r="AT24"/>
     </row>
     <row r="25" spans="3:46">
-      <c r="AJ25" s="1"/>
       <c r="AL25" s="1"/>
       <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
@@ -3869,7 +3880,6 @@
       <c r="AT25"/>
     </row>
     <row r="26" spans="3:46">
-      <c r="AJ26" s="1"/>
       <c r="AL26" s="1"/>
       <c r="AM26" s="1"/>
       <c r="AN26" s="1"/>
@@ -3880,7 +3890,6 @@
       <c r="AT26"/>
     </row>
     <row r="27" spans="3:46">
-      <c r="AJ27" s="1"/>
       <c r="AL27" s="1"/>
       <c r="AM27" s="1"/>
       <c r="AN27" s="1"/>
@@ -3902,9 +3911,10 @@
       <c r="AT28"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:I4"/>
     <mergeCell ref="AJ10:AP10"/>
-    <mergeCell ref="J3:AH3"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="O4:R4"/>
     <mergeCell ref="T4:V4"/>
@@ -3912,8 +3922,8 @@
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AE4:AH4"/>
     <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J3:R3"/>
+    <mergeCell ref="S3:AH3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3924,7 +3934,7 @@
   <dimension ref="B2:AT28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4075,82 +4085,82 @@
       <c r="I3" s="5">
         <v>0</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="23"/>
-      <c r="AH3" s="23"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
     </row>
     <row r="4" spans="2:42">
       <c r="B4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
       <c r="J4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="K4" s="1">
         <v>1</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="22"/>
+      <c r="M4" s="37"/>
       <c r="N4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22" t="s">
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22" t="s">
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
       <c r="AJ4" t="s">
         <v>96</v>
       </c>
@@ -4159,48 +4169,48 @@
       <c r="B5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
       <c r="N5" s="1">
         <v>1</v>
       </c>
-      <c r="O5" s="22" t="s">
+      <c r="O5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22" t="s">
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="22" t="s">
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="X5" s="22"/>
-      <c r="Y5" s="22"/>
-      <c r="Z5" s="22"/>
-      <c r="AA5" s="22"/>
-      <c r="AB5" s="22"/>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="22"/>
-      <c r="AE5" s="22"/>
-      <c r="AF5" s="22"/>
-      <c r="AG5" s="22"/>
-      <c r="AH5" s="22"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
+      <c r="AA5" s="37"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37"/>
+      <c r="AD5" s="37"/>
+      <c r="AE5" s="37"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="37"/>
+      <c r="AH5" s="37"/>
       <c r="AJ5" t="s">
         <v>63</v>
       </c>
@@ -4209,48 +4219,48 @@
       <c r="B6" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
       <c r="J6" s="1">
         <v>0</v>
       </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
       <c r="N6" s="1">
         <v>0</v>
       </c>
-      <c r="O6" s="22" t="s">
+      <c r="O6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22" t="s">
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22" t="s">
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="22"/>
-      <c r="AG6" s="22"/>
-      <c r="AH6" s="22"/>
+      <c r="X6" s="37"/>
+      <c r="Y6" s="37"/>
+      <c r="Z6" s="37"/>
+      <c r="AA6" s="37"/>
+      <c r="AB6" s="37"/>
+      <c r="AC6" s="37"/>
+      <c r="AD6" s="37"/>
+      <c r="AE6" s="37"/>
+      <c r="AF6" s="37"/>
+      <c r="AG6" s="37"/>
+      <c r="AH6" s="37"/>
       <c r="AJ6" t="s">
         <v>64</v>
       </c>
@@ -4277,15 +4287,15 @@
     </row>
     <row r="9" spans="2:42" ht="15.75" thickBot="1"/>
     <row r="10" spans="2:42" ht="15.75" thickBot="1">
-      <c r="AJ10" s="24" t="s">
+      <c r="AJ10" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="AK10" s="25"/>
-      <c r="AL10" s="25"/>
-      <c r="AM10" s="25"/>
-      <c r="AN10" s="25"/>
-      <c r="AO10" s="25"/>
-      <c r="AP10" s="26"/>
+      <c r="AK10" s="41"/>
+      <c r="AL10" s="41"/>
+      <c r="AM10" s="41"/>
+      <c r="AN10" s="41"/>
+      <c r="AO10" s="41"/>
+      <c r="AP10" s="42"/>
     </row>
     <row r="11" spans="2:42" ht="15.75" thickBot="1">
       <c r="AJ11" s="17" t="s">
@@ -4450,74 +4460,74 @@
       <c r="N16" s="1">
         <v>1</v>
       </c>
-      <c r="O16" s="31">
-        <v>0</v>
-      </c>
-      <c r="P16" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="32">
-        <v>0</v>
-      </c>
-      <c r="R16" s="32">
-        <v>1</v>
-      </c>
-      <c r="S16" s="30">
-        <v>0</v>
-      </c>
-      <c r="T16" s="30">
-        <v>0</v>
-      </c>
-      <c r="U16" s="30">
-        <v>1</v>
-      </c>
-      <c r="V16" s="30">
-        <v>0</v>
-      </c>
-      <c r="W16" s="35">
-        <v>0</v>
-      </c>
-      <c r="X16" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AF16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="33" t="s">
+      <c r="O16" s="26">
+        <v>0</v>
+      </c>
+      <c r="P16" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="27">
+        <v>0</v>
+      </c>
+      <c r="R16" s="27">
+        <v>1</v>
+      </c>
+      <c r="S16" s="25">
+        <v>0</v>
+      </c>
+      <c r="T16" s="25">
+        <v>0</v>
+      </c>
+      <c r="U16" s="25">
+        <v>1</v>
+      </c>
+      <c r="V16" s="25">
+        <v>0</v>
+      </c>
+      <c r="W16" s="30">
+        <v>0</v>
+      </c>
+      <c r="X16" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="AJ16" s="34" t="s">
+      <c r="AJ16" s="29" t="s">
         <v>108</v>
       </c>
       <c r="AK16" s="8"/>
-      <c r="AL16" s="27" t="s">
+      <c r="AL16" s="22" t="s">
         <v>97</v>
       </c>
       <c r="AM16" s="9"/>
@@ -4526,10 +4536,10 @@
       <c r="AP16" s="8"/>
     </row>
     <row r="17" spans="2:46">
-      <c r="AI17" s="33"/>
-      <c r="AJ17" s="34"/>
+      <c r="AI17" s="28"/>
+      <c r="AJ17" s="29"/>
       <c r="AK17" s="8"/>
-      <c r="AL17" s="27" t="s">
+      <c r="AL17" s="22" t="s">
         <v>98</v>
       </c>
       <c r="AM17" s="9"/>
@@ -4577,74 +4587,74 @@
       <c r="N18" s="2">
         <v>0</v>
       </c>
-      <c r="O18" s="31">
-        <v>0</v>
-      </c>
-      <c r="P18" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="32">
-        <v>1</v>
-      </c>
-      <c r="R18" s="32">
-        <v>0</v>
-      </c>
-      <c r="S18" s="30">
-        <v>0</v>
-      </c>
-      <c r="T18" s="30">
-        <v>0</v>
-      </c>
-      <c r="U18" s="30">
-        <v>1</v>
-      </c>
-      <c r="V18" s="30">
-        <v>1</v>
-      </c>
-      <c r="W18" s="35">
-        <v>0</v>
-      </c>
-      <c r="X18" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="35">
-        <v>1</v>
-      </c>
-      <c r="AH18" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI18" s="33" t="s">
+      <c r="O18" s="26">
+        <v>0</v>
+      </c>
+      <c r="P18" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="27">
+        <v>1</v>
+      </c>
+      <c r="R18" s="27">
+        <v>0</v>
+      </c>
+      <c r="S18" s="25">
+        <v>0</v>
+      </c>
+      <c r="T18" s="25">
+        <v>0</v>
+      </c>
+      <c r="U18" s="25">
+        <v>1</v>
+      </c>
+      <c r="V18" s="25">
+        <v>1</v>
+      </c>
+      <c r="W18" s="30">
+        <v>0</v>
+      </c>
+      <c r="X18" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="30">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="AJ18" s="34" t="s">
+      <c r="AJ18" s="29" t="s">
         <v>110</v>
       </c>
       <c r="AK18" s="8"/>
-      <c r="AL18" s="27" t="s">
+      <c r="AL18" s="22" t="s">
         <v>99</v>
       </c>
       <c r="AM18" s="9"/>
@@ -4653,15 +4663,15 @@
       <c r="AP18" s="8"/>
     </row>
     <row r="19" spans="2:46">
-      <c r="AI19" s="33"/>
-      <c r="AJ19" s="34"/>
+      <c r="AI19" s="28"/>
+      <c r="AJ19" s="29"/>
       <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
       <c r="AO19" s="1"/>
     </row>
     <row r="20" spans="2:46">
       <c r="B20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -4692,9 +4702,9 @@
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
-      <c r="AI20" s="33"/>
-      <c r="AJ20" s="34"/>
-      <c r="AL20" s="27" t="s">
+      <c r="AI20" s="28"/>
+      <c r="AJ20" s="29"/>
+      <c r="AL20" s="22" t="s">
         <v>101</v>
       </c>
       <c r="AM20" s="1"/>
@@ -4707,7 +4717,7 @@
     </row>
     <row r="21" spans="2:46">
       <c r="B21" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -4735,9 +4745,9 @@
       <c r="AF21" s="3"/>
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
-      <c r="AI21" s="33"/>
-      <c r="AJ21" s="34"/>
-      <c r="AL21" s="27" t="s">
+      <c r="AI21" s="28"/>
+      <c r="AJ21" s="29"/>
+      <c r="AL21" s="22" t="s">
         <v>102</v>
       </c>
       <c r="AM21" s="1"/>
@@ -4776,8 +4786,8 @@
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
-      <c r="AI22" s="33"/>
-      <c r="AJ22" s="34"/>
+      <c r="AI22" s="28"/>
+      <c r="AJ22" s="29"/>
       <c r="AL22" s="1"/>
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
@@ -4788,8 +4798,8 @@
       <c r="AT22"/>
     </row>
     <row r="23" spans="2:46">
-      <c r="AI23" s="33"/>
-      <c r="AJ23" s="34"/>
+      <c r="AI23" s="28"/>
+      <c r="AJ23" s="29"/>
       <c r="AL23" s="1"/>
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
@@ -4800,8 +4810,8 @@
       <c r="AT23"/>
     </row>
     <row r="24" spans="2:46">
-      <c r="AI24" s="33"/>
-      <c r="AJ24" s="34"/>
+      <c r="AI24" s="28"/>
+      <c r="AJ24" s="29"/>
       <c r="AL24" s="1"/>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
@@ -4812,8 +4822,8 @@
       <c r="AT24"/>
     </row>
     <row r="25" spans="2:46">
-      <c r="AI25" s="33"/>
-      <c r="AJ25" s="34"/>
+      <c r="AI25" s="28"/>
+      <c r="AJ25" s="29"/>
       <c r="AL25" s="1"/>
       <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
@@ -4824,8 +4834,8 @@
       <c r="AT25"/>
     </row>
     <row r="26" spans="2:46">
-      <c r="AI26" s="33"/>
-      <c r="AJ26" s="34"/>
+      <c r="AI26" s="28"/>
+      <c r="AJ26" s="29"/>
       <c r="AL26" s="1"/>
       <c r="AM26" s="1"/>
       <c r="AN26" s="1"/>
@@ -4836,8 +4846,8 @@
       <c r="AT26"/>
     </row>
     <row r="27" spans="2:46">
-      <c r="AI27" s="33"/>
-      <c r="AJ27" s="34"/>
+      <c r="AI27" s="28"/>
+      <c r="AJ27" s="29"/>
       <c r="AL27" s="1"/>
       <c r="AM27" s="1"/>
       <c r="AN27" s="1"/>
@@ -4859,8 +4869,7 @@
       <c r="AT28"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="J3:AH3"/>
+  <mergeCells count="16">
     <mergeCell ref="O4:R4"/>
     <mergeCell ref="O5:R5"/>
     <mergeCell ref="S5:V5"/>
@@ -4870,11 +4879,13 @@
     <mergeCell ref="W6:AH6"/>
     <mergeCell ref="L5:M6"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="C4:I6"/>
+    <mergeCell ref="J3:R3"/>
+    <mergeCell ref="S3:AH3"/>
     <mergeCell ref="AJ10:AP10"/>
     <mergeCell ref="W4:AH4"/>
     <mergeCell ref="S4:V4"/>
     <mergeCell ref="L4:M4"/>
+    <mergeCell ref="C4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4885,7 +4896,7 @@
   <dimension ref="B2:AT28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF20" sqref="AF20"/>
+      <selection activeCell="I5" sqref="I5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5026,61 +5037,61 @@
       <c r="G3" s="5">
         <v>0</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
       <c r="S3" s="5">
         <v>1</v>
       </c>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="23"/>
-      <c r="AH3" s="23"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
     </row>
     <row r="4" spans="2:46">
       <c r="B4" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
       <c r="T4" s="1">
         <v>0</v>
       </c>
@@ -5093,19 +5104,19 @@
       <c r="W4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="X4" s="22" t="s">
+      <c r="X4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="22"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="22"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
       <c r="AJ4" s="3" t="s">
         <v>100</v>
       </c>
@@ -5117,29 +5128,29 @@
       <c r="B5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
       <c r="H5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22" t="s">
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
       <c r="T5" s="1">
         <v>0</v>
       </c>
@@ -5152,19 +5163,19 @@
       <c r="W5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="X5" s="22" t="s">
+      <c r="X5" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="Y5" s="22"/>
-      <c r="Z5" s="22"/>
-      <c r="AA5" s="22"/>
-      <c r="AB5" s="22"/>
-      <c r="AC5" s="22"/>
-      <c r="AD5" s="22"/>
-      <c r="AE5" s="22"/>
-      <c r="AF5" s="22"/>
-      <c r="AG5" s="22"/>
-      <c r="AH5" s="22"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
+      <c r="AA5" s="37"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37"/>
+      <c r="AD5" s="37"/>
+      <c r="AE5" s="37"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="37"/>
+      <c r="AH5" s="37"/>
       <c r="AJ5" t="s">
         <v>85</v>
       </c>
@@ -5256,111 +5267,111 @@
     </row>
     <row r="15" spans="2:46">
       <c r="B15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="30">
+        <v>0</v>
+      </c>
+      <c r="J15" s="30">
+        <v>0</v>
+      </c>
+      <c r="K15" s="30">
+        <v>0</v>
+      </c>
+      <c r="L15" s="30">
+        <v>0</v>
+      </c>
+      <c r="M15" s="30">
+        <v>0</v>
+      </c>
+      <c r="N15" s="30">
+        <v>0</v>
+      </c>
+      <c r="O15" s="30">
+        <v>0</v>
+      </c>
+      <c r="P15" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="30">
+        <v>0</v>
+      </c>
+      <c r="R15" s="30">
+        <v>0</v>
+      </c>
+      <c r="S15" s="6">
+        <v>1</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0</v>
+      </c>
+      <c r="U15" s="30">
+        <v>0</v>
+      </c>
+      <c r="V15" s="1">
+        <v>1</v>
+      </c>
+      <c r="W15" s="30">
+        <v>0</v>
+      </c>
+      <c r="X15" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="30">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="30">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ15" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="6">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6">
-        <v>1</v>
-      </c>
-      <c r="F15" s="6">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="35">
-        <v>0</v>
-      </c>
-      <c r="J15" s="35">
-        <v>0</v>
-      </c>
-      <c r="K15" s="35">
-        <v>0</v>
-      </c>
-      <c r="L15" s="35">
-        <v>0</v>
-      </c>
-      <c r="M15" s="35">
-        <v>0</v>
-      </c>
-      <c r="N15" s="35">
-        <v>0</v>
-      </c>
-      <c r="O15" s="35">
-        <v>0</v>
-      </c>
-      <c r="P15" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="35">
-        <v>0</v>
-      </c>
-      <c r="R15" s="35">
-        <v>0</v>
-      </c>
-      <c r="S15" s="6">
-        <v>1</v>
-      </c>
-      <c r="T15" s="1">
-        <v>0</v>
-      </c>
-      <c r="U15" s="35">
-        <v>0</v>
-      </c>
-      <c r="V15" s="1">
-        <v>1</v>
-      </c>
-      <c r="W15" s="35">
-        <v>0</v>
-      </c>
-      <c r="X15" s="35">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="35">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="35">
-        <v>1</v>
-      </c>
-      <c r="AA15" s="35">
-        <v>1</v>
-      </c>
-      <c r="AB15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="35">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="AJ15" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK15" s="28"/>
+      <c r="AK15" s="23"/>
       <c r="AL15" s="9"/>
       <c r="AM15" s="9"/>
       <c r="AN15" s="9"/>
@@ -5500,16 +5511,17 @@
       <c r="AT28"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="X5:AH5"/>
     <mergeCell ref="S4:S5"/>
-    <mergeCell ref="C4:G5"/>
     <mergeCell ref="H3:R3"/>
     <mergeCell ref="T3:AH3"/>
     <mergeCell ref="I4:R4"/>
     <mergeCell ref="X4:AH4"/>
     <mergeCell ref="I5:L5"/>
     <mergeCell ref="M5:R5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>